<commit_message>
agenda and apeaker import changes in field name
</commit_message>
<xml_diff>
--- a/public/agenda_sample.xlsx
+++ b/public/agenda_sample.xlsx
@@ -26,7 +26,7 @@
     <t>Speaker</t>
   </si>
   <si>
-    <t>Start Date</t>
+    <t>Start Date DD/MM/YYYY</t>
   </si>
   <si>
     <t>Start Time Hour</t>
@@ -38,7 +38,7 @@
     <t>Start Time AM/PM</t>
   </si>
   <si>
-    <t>End Date</t>
+    <t>End Date DD/MM/YYYY</t>
   </si>
   <si>
     <t>End Time Hour</t>
@@ -80,7 +80,7 @@
     <t>PM</t>
   </si>
   <si>
-    <t>active</t>
+    <t>Active / deactive</t>
   </si>
 </sst>
 </file>
@@ -156,12 +156,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -193,93 +189,93 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="2" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>